<commit_message>
Correzzione errori come da indicazioni relative all'ultimo tentativo di accreditamento fallito.
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/accreditamento-checklist_V8.1.2.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.0/accreditamento-checklist_V8.1.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insiel.sharepoint.com/sites/O365-Clinico/Documenti condivisi/PNRR-FSE- Indicatori e  CDA2-Clinico Cardiologia SEI/Clinico/Accreditamento/Documenti da spedire 2023 03 17/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insiel.sharepoint.com/sites/O365-Clinico/Documenti condivisi/PNRR-FSE- Indicatori e  CDA2-Clinico Cardiologia SEI/Clinico/Accreditamento/Documenti da spedire 2023 03 31/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="8_{F5F8808C-9FE5-4EEA-A5E4-1FF1B9930C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{268F0B4D-5784-4C86-808B-129D33826F67}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="8_{F5F8808C-9FE5-4EEA-A5E4-1FF1B9930C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83D937D5-610F-433C-9B3D-39683DF4E139}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4425,31 +4425,7 @@
     <t>subject_application_version: G4.3.0</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:08:01</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:08:01Z</t>
-  </si>
-  <si>
-    <t>16b038a81e3d2a9e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.e498a5183d7499a6268b8d9a21dae59a4736d08c9e3fb11268da1d8158f9a734.b43f06bb6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>I DATI OPZIONALI RICHIESTI NON SONO GESTITI DALL'APPLICATIVO</t>
-  </si>
-  <si>
-    <t>31d7c04efb2e0841</t>
-  </si>
-  <si>
-    <t>Tue,21 Mar 2023 14:09:53</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:09:53Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.1498a06ae897f82aeca7468a7355e74218963ebed0c8432c3da6282486c8ac63.b9f9ddd06f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">3) Se il test è applicabile la colonna APPLICABILITA' deve essere compilata con SI e dovranno essere valorizzate:
@@ -4469,34 +4445,10 @@
   "detail": "ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected."</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:10:34</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:10:34Z</t>
-  </si>
-  <si>
-    <t>3dc0e47690aab16c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.e498a5183d7499a6268b8d9a21dae59a4736d08c9e3fb11268da1d8158f9a734.8fb987574b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 422,
   "detail": "[Errore-46| codice fiscale 'PROVAX00x00x0x' cittadino ed operatore: 16 cifre [A-Z0-9]{16}],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
   </si>
   <si>
-    <t xml:space="preserve">Tue,21 Mar 2023 14:11:24 </t>
-  </si>
-  <si>
-    <t>2023-03-21T14:11:24Z</t>
-  </si>
-  <si>
-    <t>77dfd4a765319917</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.3913314e0fcaceb3d898d5a5fff9fbd531ef6dc5e4227816ee52146c9cf70945.f08f855d6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 422,
   "detail": "[ERRORE-6| L'elemento  'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code  valorizzato con 'N' o 'V', e il suo @codeSystem  con '2.16.840.1.113883.5.25'],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
   </si>
@@ -4504,114 +4456,26 @@
     <t>L'OPERATORE PUO' RIVEDERE LE SEZIONI DI ERRORE ED EVENTUALMENTE RIVALIDA IL DOCUMENTO</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:20:03</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:20:03Z</t>
-  </si>
-  <si>
-    <t>842fdfc17612981e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.c9859ce91c83cf2833b7379b69194bba59c2ee9255ee7174626efb776079eeae.a0d9d30a2f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 422,
   "detail": "[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:20:39</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:20:39Z</t>
-  </si>
-  <si>
-    <t>ca1010c223f86976</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.1abd132b1ef685db26ea8302de934f949e867aaa7603ea6bb2fa407f55b9d847.c22398e119^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 400,
   "detail": "Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB]"</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:21:20</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:21:20Z</t>
-  </si>
-  <si>
-    <t>1f582b5e82194c33</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.7aef179fcac6514da004b6df4eebeb49d68de9d8cc51ec644f3f5061fad1cfc8.2fb7182b53^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>"status": 400,
-  "detail": "Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.2.7 v1.0.0, Codes: 0]"</t>
-  </si>
-  <si>
-    <t>Tue,21 Mar 2023 14:21:51</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:21:51Z</t>
-  </si>
-  <si>
-    <t>e586d9c65ba57ed9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.354af7828b256dbac3f1b222ff8706f6f911cfe17f2af318dd75031ca35ba097.20151657b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 422,
   "detail": "[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ],[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:22:25</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:22:25Z</t>
-  </si>
-  <si>
-    <t>a731b34eb97ba54d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.36fd1f3d5f4d79a424104d693a900c0413b61b81a5ceb3fe1079b8d12a863dea.56977330b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">  "status": 400,
   "detail": "ERROR: -1,-1 cvc-complex-type.2.4.b: The content of element 'order' is not complete. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected.,ERROR: -1,-1 cvc-complex-type.2.4.b: The content of element 'order' is not complete. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected."</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:23:08</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:23:08Z</t>
-  </si>
-  <si>
-    <t>798c85fb99ef1ab3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.1e56003d3cd270ca128b8aacdbc307a66ac12aad7c13bf7f2676bb1598e89acb.52186850a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 400,
   "detail": "ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'text'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected."</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 14:24:37</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:24:37Z</t>
-  </si>
-  <si>
-    <t>5be91f66b0140342</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.81540a0dd1700dfdcaa0d2f75c91e27f31863cdc7df3922533b397dd5672d1f1.080ca91869^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 422,
   "detail": "[ERRORE-b4| Sezione Referto: DEVE essere presente la sezione \"Referto\".],[ERRORE-b5| Sezione Referto: La sezione deve contenere l'elemento 'text'.],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica\n\t\t\tLOINC @codeSystem='2.16.840.1.113883.6.1'\n\t\t\tICD-9-CM @codeSystem='2.16.840.1.113883.6.103']"</t>
   </si>
@@ -4619,42 +4483,6 @@
     <t>TEST NON ESEGUIBILE PERCHE' SARA' OGGETTO DELL'ACCREDITAMENTO DEL MIDDLEWARE REGIONALE</t>
   </si>
   <si>
-    <t xml:space="preserve">Tue,21 Mar 2023 14:37:10 </t>
-  </si>
-  <si>
-    <t>2023-03-21T14:37:10Z</t>
-  </si>
-  <si>
-    <t>f767da9eff899fe3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.54d857015c7cb3ea6950a4564a39bb344bc3f3d9bdfcb3f58e7f9fd20af60c3e.9da00b8eb0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Tue,21 Mar 2023 14:56:51</t>
-  </si>
-  <si>
-    <t>2023-03-21T14:56:51Z</t>
-  </si>
-  <si>
-    <t>1ddda7b53836813c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.626a28918d7f7e6c6ee9abc686619849c2e3c37920575bb7b0d815cb610ab589.ccb5744f6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Tue,21 Mar 2023 15:07:10</t>
-  </si>
-  <si>
-    <t>2023-03-21T15:07:10Z</t>
-  </si>
-  <si>
-    <t>529fc7e93c873e69</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.54d857015c7cb3ea6950a4564a39bb344bc3f3d9bdfcb3f58e7f9fd20af60c3e.622c5f5992^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 422,
   "detail": "[Errore-47| codice fiscale 'PROVAX00x00x0x' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]"</t>
   </si>
@@ -4662,12 +4490,6 @@
     <t>Tue,21 Mar 2023 15:07:46</t>
   </si>
   <si>
-    <t>2023-03-21T15:07:46Z</t>
-  </si>
-  <si>
-    <t>04aec1512b4b02a9</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.60.4.4.678747fc6f63290eb3205495dc3983c2b6bf1c803ce9f3a7f68406444a2cd6d8.15e3f63dc8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -4675,46 +4497,10 @@
   "detail": "[ERRORE-6| L'elemento 'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']",</t>
   </si>
   <si>
-    <t>Tue,21 Mar 2023 15:08:20</t>
-  </si>
-  <si>
-    <t>2023-03-21T15:08:20Z</t>
-  </si>
-  <si>
-    <t>21a40ee32bcaccc0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.53d949924be68943fe98930b9c5bd8550bb322f43e24bc8de9bc2812a5345574.97493f0032^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"status": 422,
   "detail": "[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']"</t>
   </si>
   <si>
-    <t xml:space="preserve">Tue,21 Mar 2023 15:09:01 </t>
-  </si>
-  <si>
-    <t>2023-03-21T15:09:01Z</t>
-  </si>
-  <si>
-    <t>4c76652e46ef1019</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.1272f00eb9c0fe7bcc5d55445c1bfbe2d0563f559ff6cb658be6c72f063a60a3.22a3ac3b92^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Tue,21 Mar 2023 15:09:26</t>
-  </si>
-  <si>
-    <t>2023-03-21T15:09:26Z</t>
-  </si>
-  <si>
-    <t>7b3ddc14491bdf6d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.94d73786a78a708c64faa8cf649081f6089ad95afdd107aacd23b21a6ecc5b08.50b6fcc896^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>"detail": "[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]"</t>
   </si>
   <si>
@@ -4722,12 +4508,6 @@
   </si>
   <si>
     <t>2023-03-21T15:09:48Z</t>
-  </si>
-  <si>
-    <t>a7b6a7c8d274e537</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.e194fba4d5beb729d2851f835083f014c36ea7480fb3a6f8e9d43f5e5acd365a.5911a345ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>"status": 422,
@@ -4737,6 +4517,226 @@
     <t>"status": 504,
 "detail": la richiesta al gateway è andata in timeout
 La procedura consiste nella rivalidazione del documento quando il servizio ritorna disponibile</t>
+  </si>
+  <si>
+    <t>999265a510fc446f</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 11:11:29</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.54d857015c7cb3ea6950a4564a39bb344bc3f3d9bdfcb3f58e7f9fd20af60c3e.0d02dc7d1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 11:12:16</t>
+  </si>
+  <si>
+    <t>2023-03-31T11:12:16Z</t>
+  </si>
+  <si>
+    <t>99b88333d9e596d5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.626a28918d7f7e6c6ee9abc686619849c2e3c37920575bb7b0d815cb610ab589.998975ab1a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>TFri,31 Mar 2023 11:14:13</t>
+  </si>
+  <si>
+    <t>2023-03-31T11:14:13Z</t>
+  </si>
+  <si>
+    <t>5b4395bf7f3a5782</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.54d857015c7cb3ea6950a4564a39bb344bc3f3d9bdfcb3f58e7f9fd20af60c3e.cac92bacfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 11:15:09</t>
+  </si>
+  <si>
+    <t>494935524c2bb848</t>
+  </si>
+  <si>
+    <t>a6dca3677abf7b7a</t>
+  </si>
+  <si>
+    <t>2023-03-31T11:15:09Z</t>
+  </si>
+  <si>
+    <t>2023-03-31T15:07:46Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.53d949924be68943fe98930b9c5bd8550bb322f43e24bc8de9bc2812a5345574.11222007f1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 11:16:00</t>
+  </si>
+  <si>
+    <t>2023-03-31T11:16:00Z</t>
+  </si>
+  <si>
+    <t>dd2935138ba8fcad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.1272f00eb9c0fe7bcc5d55445c1bfbe2d0563f559ff6cb658be6c72f063a60a3.3be30287a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1a99c32c40b7365d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.94d73786a78a708c64faa8cf649081f6089ad95afdd107aacd23b21a6ecc5b08.8d7eb53194^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>: Fri,31 Mar 2023 11:16:40</t>
+  </si>
+  <si>
+    <t>2023-03-31T11:16:40Z</t>
+  </si>
+  <si>
+    <t>60084174a4b38246</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.e194fba4d5beb729d2851f835083f014c36ea7480fb3a6f8e9d43f5e5acd365a.4ea4762b38^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>045c7e424f9a11ba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.e498a5183d7499a6268b8d9a21dae59a4736d08c9e3fb11268da1d8158f9a734.8618b90ee2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">: Fri,31 Mar 2023 12:04:42 </t>
+  </si>
+  <si>
+    <t>2023-03-31T12:04:42Z</t>
+  </si>
+  <si>
+    <t>dac21473b21770ea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.1498a06ae897f82aeca7468a7355e74218963ebed0c8432c3da6282486c8ac63.eab7162cd1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 12:06:57</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:06:57Z</t>
+  </si>
+  <si>
+    <t>: Fri,31 Mar 2023 12:10:29</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:10:29Z</t>
+  </si>
+  <si>
+    <t>c3973e855922a6bb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.e498a5183d7499a6268b8d9a21dae59a4736d08c9e3fb11268da1d8158f9a734.3348e88f23^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri,31 Mar 2023 12:10:58 </t>
+  </si>
+  <si>
+    <t>2023-03-31T12:10:58Z</t>
+  </si>
+  <si>
+    <t>2d08800cbd1b45f3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.3913314e0fcaceb3d898d5a5fff9fbd531ef6dc5e4227816ee52146c9cf70945.85c9ebe7a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 12:12:46</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:12:46Z</t>
+  </si>
+  <si>
+    <t>9b828eb36b18fccf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.c9859ce91c83cf2833b7379b69194bba59c2ee9255ee7174626efb776079eeae.6fccf273f2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 12:14:28</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:14:28Z</t>
+  </si>
+  <si>
+    <t>f30d8187028b03cb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.1abd132b1ef685db26ea8302de934f949e867aaa7603ea6bb2fa407f55b9d847.d5451d2d84^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 12:15:26</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:15:26Z</t>
+  </si>
+  <si>
+    <t>c5e4b1a97a9fd612</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.354af7828b256dbac3f1b222ff8706f6f911cfe17f2af318dd75031ca35ba097.5934820244^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>dc191743967203a9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.36fd1f3d5f4d79a424104d693a900c0413b61b81a5ceb3fe1079b8d12a863dea.6ec22064ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>: Fri,31 Mar 2023 12:15:57</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:15:57Z</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 12:16:36</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:16:36Z</t>
+  </si>
+  <si>
+    <t>a264b9439aa435e5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.1e56003d3cd270ca128b8aacdbc307a66ac12aad7c13bf7f2676bb1598e89acb.8f9500228a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fri,31 Mar 2023 12:18:09</t>
+  </si>
+  <si>
+    <t>2023-03-31T12:18:09Z</t>
+  </si>
+  <si>
+    <t>4fbcab6c6e9e9973</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.81540a0dd1700dfdcaa0d2f75c91e27f31863cdc7df3922533b397dd5672d1f1.271dea5a20^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-31T11:11:29Z</t>
+  </si>
+  <si>
+    <t>600faeb4870f7025</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.7aef179fcac6514da004b6df4eebeb49d68de9d8cc51ec644f3f5061fad1cfc8.c43b28b1a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Mon,03 Apr 2023 06:26:26</t>
+  </si>
+  <si>
+    <t>2023-04-03T06:26:26Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "status": 400,
+  "detail": "Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.2.7 v1.0.0, Codes: XX]"</t>
   </si>
 </sst>
 </file>
@@ -5062,7 +5062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5164,6 +5164,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -5511,7 +5514,7 @@
     </row>
     <row r="4" spans="1:1" ht="14.25" customHeight="1">
       <c r="A4" s="36" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.25" customHeight="1">
@@ -7648,11 +7651,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="H212" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="D264" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M212" sqref="M212"/>
+      <selection pane="bottomRight" activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7691,14 +7694,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>829</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7716,14 +7719,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>831</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="50"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7741,12 +7744,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="48" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>830</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7765,12 +7768,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>832</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="50"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -14062,7 +14065,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="150.75" thickBot="1">
+    <row r="191" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A191" s="20">
         <v>6</v>
       </c>
@@ -14079,16 +14082,16 @@
         <v>415</v>
       </c>
       <c r="F191" s="35" t="s">
-        <v>891</v>
-      </c>
-      <c r="G191" s="24" t="s">
-        <v>892</v>
+        <v>857</v>
+      </c>
+      <c r="G191" s="34" t="s">
+        <v>923</v>
       </c>
       <c r="H191" s="24" t="s">
-        <v>893</v>
+        <v>856</v>
       </c>
       <c r="I191" s="24" t="s">
-        <v>894</v>
+        <v>858</v>
       </c>
       <c r="J191" s="25" t="s">
         <v>488</v>
@@ -14108,7 +14111,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="150.75" thickBot="1">
+    <row r="192" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A192" s="20">
         <v>7</v>
       </c>
@@ -14132,7 +14135,7 @@
         <v>828</v>
       </c>
       <c r="K192" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L192" s="25"/>
       <c r="M192" s="25"/>
@@ -14146,7 +14149,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="150.75" thickBot="1">
+    <row r="193" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A193" s="20">
         <v>8</v>
       </c>
@@ -14170,7 +14173,7 @@
         <v>828</v>
       </c>
       <c r="K193" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L193" s="25"/>
       <c r="M193" s="25"/>
@@ -14184,7 +14187,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="150.75" thickBot="1">
+    <row r="194" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A194" s="20">
         <v>9</v>
       </c>
@@ -14208,7 +14211,7 @@
         <v>828</v>
       </c>
       <c r="K194" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L194" s="25"/>
       <c r="M194" s="25"/>
@@ -14238,17 +14241,17 @@
       <c r="E195" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="F195" s="23" t="s">
-        <v>833</v>
+      <c r="F195" s="35" t="s">
+        <v>885</v>
       </c>
       <c r="G195" s="34" t="s">
-        <v>834</v>
-      </c>
-      <c r="H195" s="24" t="s">
-        <v>835</v>
-      </c>
-      <c r="I195" s="24" t="s">
-        <v>836</v>
+        <v>886</v>
+      </c>
+      <c r="H195" s="34" t="s">
+        <v>883</v>
+      </c>
+      <c r="I195" s="34" t="s">
+        <v>884</v>
       </c>
       <c r="J195" s="25" t="s">
         <v>488</v>
@@ -14292,7 +14295,7 @@
         <v>828</v>
       </c>
       <c r="K196" s="37" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L196" s="25"/>
       <c r="M196" s="25"/>
@@ -14330,7 +14333,7 @@
         <v>828</v>
       </c>
       <c r="K197" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L197" s="25"/>
       <c r="M197" s="25"/>
@@ -14368,7 +14371,7 @@
         <v>828</v>
       </c>
       <c r="K198" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
@@ -14824,7 +14827,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="150.75" thickBot="1">
+    <row r="212" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A212" s="20">
         <v>29</v>
       </c>
@@ -14848,7 +14851,7 @@
         <v>828</v>
       </c>
       <c r="K212" s="25" t="s">
-        <v>890</v>
+        <v>845</v>
       </c>
       <c r="L212" s="25"/>
       <c r="M212" s="25"/>
@@ -14920,7 +14923,7 @@
         <v>828</v>
       </c>
       <c r="K214" s="25" t="s">
-        <v>890</v>
+        <v>845</v>
       </c>
       <c r="L214" s="25"/>
       <c r="M214" s="25"/>
@@ -15104,7 +15107,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="165.75" thickBot="1">
+    <row r="220" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A220" s="20">
         <v>37</v>
       </c>
@@ -15128,7 +15131,7 @@
         <v>828</v>
       </c>
       <c r="K220" s="25" t="s">
-        <v>890</v>
+        <v>845</v>
       </c>
       <c r="L220" s="25"/>
       <c r="M220" s="25"/>
@@ -15200,7 +15203,7 @@
         <v>828</v>
       </c>
       <c r="K222" s="37" t="s">
-        <v>890</v>
+        <v>845</v>
       </c>
       <c r="L222" s="25"/>
       <c r="M222" s="25"/>
@@ -15386,7 +15389,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="105.75" thickBot="1">
+    <row r="228" spans="1:20" ht="105.75" hidden="1" thickBot="1">
       <c r="A228" s="20">
         <v>45</v>
       </c>
@@ -15413,7 +15416,7 @@
       <c r="N228" s="25"/>
       <c r="O228" s="25"/>
       <c r="P228" s="25" t="s">
-        <v>928</v>
+        <v>855</v>
       </c>
       <c r="Q228" s="25"/>
       <c r="R228" s="26" t="s">
@@ -15487,7 +15490,7 @@
       <c r="N230" s="25"/>
       <c r="O230" s="25"/>
       <c r="P230" s="25" t="s">
-        <v>928</v>
+        <v>855</v>
       </c>
       <c r="Q230" s="25"/>
       <c r="R230" s="26" t="s">
@@ -16016,7 +16019,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="120.75" thickBot="1">
+    <row r="246" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A246" s="20">
         <v>63</v>
       </c>
@@ -16033,16 +16036,16 @@
         <v>519</v>
       </c>
       <c r="F246" s="35" t="s">
-        <v>895</v>
+        <v>859</v>
       </c>
       <c r="G246" s="34" t="s">
-        <v>896</v>
+        <v>860</v>
       </c>
       <c r="H246" s="34" t="s">
-        <v>897</v>
+        <v>861</v>
       </c>
       <c r="I246" s="34" t="s">
-        <v>898</v>
+        <v>862</v>
       </c>
       <c r="J246" s="25" t="s">
         <v>488</v>
@@ -16055,13 +16058,13 @@
         <v>488</v>
       </c>
       <c r="N246" s="37" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="O246" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P246" s="37" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q246" s="37" t="s">
         <v>826</v>
@@ -16072,7 +16075,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="120.75" thickBot="1">
+    <row r="247" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A247" s="20">
         <v>64</v>
       </c>
@@ -16089,16 +16092,16 @@
         <v>521</v>
       </c>
       <c r="F247" s="35" t="s">
-        <v>899</v>
+        <v>863</v>
       </c>
       <c r="G247" s="34" t="s">
-        <v>900</v>
+        <v>864</v>
       </c>
       <c r="H247" s="34" t="s">
-        <v>901</v>
+        <v>865</v>
       </c>
       <c r="I247" s="34" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="J247" s="25" t="s">
         <v>488</v>
@@ -16111,13 +16114,13 @@
         <v>488</v>
       </c>
       <c r="N247" s="37" t="s">
-        <v>903</v>
+        <v>846</v>
       </c>
       <c r="O247" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P247" s="37" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q247" s="37" t="s">
         <v>826</v>
@@ -16128,7 +16131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="120.75" thickBot="1">
+    <row r="248" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A248" s="20">
         <v>65</v>
       </c>
@@ -16145,16 +16148,16 @@
         <v>523</v>
       </c>
       <c r="F248" s="35" t="s">
-        <v>904</v>
+        <v>847</v>
       </c>
       <c r="G248" s="34" t="s">
-        <v>905</v>
+        <v>871</v>
       </c>
       <c r="H248" s="34" t="s">
-        <v>906</v>
+        <v>868</v>
       </c>
       <c r="I248" s="34" t="s">
-        <v>907</v>
+        <v>848</v>
       </c>
       <c r="J248" s="25" t="s">
         <v>488</v>
@@ -16167,13 +16170,13 @@
         <v>488</v>
       </c>
       <c r="N248" s="37" t="s">
-        <v>908</v>
+        <v>849</v>
       </c>
       <c r="O248" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P248" s="37" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q248" s="25" t="s">
         <v>826</v>
@@ -16184,7 +16187,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="120.75" thickBot="1">
+    <row r="249" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A249" s="20">
         <v>66</v>
       </c>
@@ -16208,7 +16211,7 @@
         <v>828</v>
       </c>
       <c r="K249" s="37" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L249" s="25"/>
       <c r="M249" s="25"/>
@@ -16222,7 +16225,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="120.75" thickBot="1">
+    <row r="250" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A250" s="20">
         <v>67</v>
       </c>
@@ -16239,16 +16242,16 @@
         <v>527</v>
       </c>
       <c r="F250" s="35" t="s">
-        <v>909</v>
+        <v>867</v>
       </c>
       <c r="G250" s="34" t="s">
-        <v>910</v>
+        <v>870</v>
       </c>
       <c r="H250" s="34" t="s">
-        <v>911</v>
+        <v>869</v>
       </c>
       <c r="I250" s="34" t="s">
-        <v>912</v>
+        <v>872</v>
       </c>
       <c r="J250" s="25" t="s">
         <v>488</v>
@@ -16261,13 +16264,13 @@
         <v>488</v>
       </c>
       <c r="N250" s="37" t="s">
-        <v>913</v>
+        <v>850</v>
       </c>
       <c r="O250" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P250" s="37" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q250" s="37" t="s">
         <v>826</v>
@@ -16278,7 +16281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="120.75" thickBot="1">
+    <row r="251" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A251" s="20">
         <v>68</v>
       </c>
@@ -16295,16 +16298,16 @@
         <v>529</v>
       </c>
       <c r="F251" s="35" t="s">
-        <v>914</v>
+        <v>873</v>
       </c>
       <c r="G251" s="34" t="s">
-        <v>915</v>
+        <v>874</v>
       </c>
       <c r="H251" s="34" t="s">
-        <v>916</v>
+        <v>875</v>
       </c>
       <c r="I251" s="34" t="s">
-        <v>917</v>
+        <v>876</v>
       </c>
       <c r="J251" s="25" t="s">
         <v>488</v>
@@ -16317,13 +16320,13 @@
         <v>488</v>
       </c>
       <c r="N251" s="37" t="s">
-        <v>864</v>
+        <v>840</v>
       </c>
       <c r="O251" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P251" s="37" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q251" s="37" t="s">
         <v>826</v>
@@ -16334,7 +16337,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="150.75" thickBot="1">
+    <row r="252" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A252" s="20">
         <v>69</v>
       </c>
@@ -16351,16 +16354,16 @@
         <v>531</v>
       </c>
       <c r="F252" s="35" t="s">
-        <v>918</v>
+        <v>879</v>
       </c>
       <c r="G252" s="34" t="s">
-        <v>919</v>
+        <v>880</v>
       </c>
       <c r="H252" s="34" t="s">
-        <v>920</v>
+        <v>877</v>
       </c>
       <c r="I252" s="34" t="s">
-        <v>921</v>
+        <v>878</v>
       </c>
       <c r="J252" s="25" t="s">
         <v>488</v>
@@ -16373,13 +16376,13 @@
         <v>488</v>
       </c>
       <c r="N252" s="37" t="s">
-        <v>922</v>
+        <v>851</v>
       </c>
       <c r="O252" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P252" s="37" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q252" s="25" t="s">
         <v>826</v>
@@ -16390,7 +16393,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="120.75" thickBot="1">
+    <row r="253" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A253" s="20">
         <v>70</v>
       </c>
@@ -16407,16 +16410,16 @@
         <v>533</v>
       </c>
       <c r="F253" s="23" t="s">
-        <v>923</v>
+        <v>852</v>
       </c>
       <c r="G253" s="24" t="s">
-        <v>924</v>
-      </c>
-      <c r="H253" s="24" t="s">
-        <v>925</v>
-      </c>
-      <c r="I253" s="24" t="s">
-        <v>926</v>
+        <v>853</v>
+      </c>
+      <c r="H253" s="34" t="s">
+        <v>881</v>
+      </c>
+      <c r="I253" s="34" t="s">
+        <v>882</v>
       </c>
       <c r="J253" s="25" t="s">
         <v>488</v>
@@ -16429,13 +16432,13 @@
         <v>488</v>
       </c>
       <c r="N253" s="25" t="s">
-        <v>927</v>
+        <v>854</v>
       </c>
       <c r="O253" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P253" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q253" s="25" t="s">
         <v>826</v>
@@ -16446,7 +16449,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="120.75" thickBot="1">
+    <row r="254" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A254" s="20">
         <v>71</v>
       </c>
@@ -16470,7 +16473,7 @@
         <v>828</v>
       </c>
       <c r="K254" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L254" s="25"/>
       <c r="M254" s="25"/>
@@ -16484,7 +16487,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="120.75" thickBot="1">
+    <row r="255" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A255" s="20">
         <v>72</v>
       </c>
@@ -16508,7 +16511,7 @@
         <v>828</v>
       </c>
       <c r="K255" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L255" s="25"/>
       <c r="M255" s="25"/>
@@ -16522,7 +16525,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="120.75" thickBot="1">
+    <row r="256" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A256" s="20">
         <v>73</v>
       </c>
@@ -16546,7 +16549,7 @@
         <v>828</v>
       </c>
       <c r="K256" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L256" s="25"/>
       <c r="M256" s="25"/>
@@ -16560,7 +16563,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="120.75" thickBot="1">
+    <row r="257" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A257" s="20">
         <v>74</v>
       </c>
@@ -16584,7 +16587,7 @@
         <v>828</v>
       </c>
       <c r="K257" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L257" s="25"/>
       <c r="M257" s="25"/>
@@ -16615,16 +16618,16 @@
         <v>543</v>
       </c>
       <c r="F258" s="35" t="s">
-        <v>839</v>
+        <v>889</v>
       </c>
       <c r="G258" s="34" t="s">
-        <v>840</v>
+        <v>890</v>
       </c>
       <c r="H258" s="34" t="s">
-        <v>838</v>
+        <v>887</v>
       </c>
       <c r="I258" s="34" t="s">
-        <v>841</v>
+        <v>888</v>
       </c>
       <c r="J258" s="25" t="s">
         <v>488</v>
@@ -16637,13 +16640,13 @@
         <v>488</v>
       </c>
       <c r="N258" s="25" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="O258" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P258" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q258" s="25" t="s">
         <v>826</v>
@@ -16670,17 +16673,17 @@
       <c r="E259" s="22" t="s">
         <v>545</v>
       </c>
-      <c r="F259" s="23" t="s">
-        <v>844</v>
-      </c>
-      <c r="G259" s="24" t="s">
-        <v>845</v>
-      </c>
-      <c r="H259" s="24" t="s">
-        <v>846</v>
-      </c>
-      <c r="I259" s="24" t="s">
-        <v>847</v>
+      <c r="F259" s="35" t="s">
+        <v>891</v>
+      </c>
+      <c r="G259" s="34" t="s">
+        <v>892</v>
+      </c>
+      <c r="H259" s="34" t="s">
+        <v>893</v>
+      </c>
+      <c r="I259" s="34" t="s">
+        <v>894</v>
       </c>
       <c r="J259" s="25" t="s">
         <v>488</v>
@@ -16693,13 +16696,13 @@
         <v>488</v>
       </c>
       <c r="N259" s="25" t="s">
-        <v>848</v>
+        <v>836</v>
       </c>
       <c r="O259" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P259" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q259" s="25" t="s">
         <v>826</v>
@@ -16726,17 +16729,17 @@
       <c r="E260" s="22" t="s">
         <v>547</v>
       </c>
-      <c r="F260" s="23" t="s">
-        <v>849</v>
-      </c>
-      <c r="G260" s="24" t="s">
-        <v>850</v>
-      </c>
-      <c r="H260" s="24" t="s">
-        <v>851</v>
-      </c>
-      <c r="I260" s="24" t="s">
-        <v>852</v>
+      <c r="F260" s="35" t="s">
+        <v>895</v>
+      </c>
+      <c r="G260" s="34" t="s">
+        <v>896</v>
+      </c>
+      <c r="H260" s="34" t="s">
+        <v>897</v>
+      </c>
+      <c r="I260" s="34" t="s">
+        <v>898</v>
       </c>
       <c r="J260" s="25" t="s">
         <v>488</v>
@@ -16749,13 +16752,13 @@
         <v>488</v>
       </c>
       <c r="N260" s="25" t="s">
-        <v>853</v>
+        <v>837</v>
       </c>
       <c r="O260" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P260" s="37" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q260" s="25" t="s">
         <v>826</v>
@@ -16790,7 +16793,7 @@
         <v>828</v>
       </c>
       <c r="K261" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L261" s="25"/>
       <c r="M261" s="25"/>
@@ -16820,17 +16823,17 @@
       <c r="E262" s="22" t="s">
         <v>551</v>
       </c>
-      <c r="F262" s="23" t="s">
-        <v>855</v>
-      </c>
-      <c r="G262" s="24" t="s">
-        <v>856</v>
-      </c>
-      <c r="H262" s="24" t="s">
-        <v>857</v>
-      </c>
-      <c r="I262" s="24" t="s">
-        <v>858</v>
+      <c r="F262" s="35" t="s">
+        <v>899</v>
+      </c>
+      <c r="G262" s="34" t="s">
+        <v>900</v>
+      </c>
+      <c r="H262" s="34" t="s">
+        <v>901</v>
+      </c>
+      <c r="I262" s="34" t="s">
+        <v>902</v>
       </c>
       <c r="J262" s="25" t="s">
         <v>488</v>
@@ -16843,13 +16846,13 @@
         <v>488</v>
       </c>
       <c r="N262" s="25" t="s">
-        <v>859</v>
+        <v>839</v>
       </c>
       <c r="O262" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P262" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q262" s="25" t="s">
         <v>826</v>
@@ -16876,17 +16879,17 @@
       <c r="E263" s="22" t="s">
         <v>553</v>
       </c>
-      <c r="F263" s="23" t="s">
-        <v>860</v>
-      </c>
-      <c r="G263" s="24" t="s">
-        <v>861</v>
-      </c>
-      <c r="H263" s="24" t="s">
-        <v>862</v>
-      </c>
-      <c r="I263" s="24" t="s">
-        <v>863</v>
+      <c r="F263" s="35" t="s">
+        <v>903</v>
+      </c>
+      <c r="G263" s="34" t="s">
+        <v>904</v>
+      </c>
+      <c r="H263" s="34" t="s">
+        <v>905</v>
+      </c>
+      <c r="I263" s="34" t="s">
+        <v>906</v>
       </c>
       <c r="J263" s="25" t="s">
         <v>488</v>
@@ -16899,13 +16902,13 @@
         <v>488</v>
       </c>
       <c r="N263" s="25" t="s">
-        <v>864</v>
+        <v>840</v>
       </c>
       <c r="O263" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P263" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q263" s="25" t="s">
         <v>826</v>
@@ -16932,17 +16935,17 @@
       <c r="E264" s="22" t="s">
         <v>555</v>
       </c>
-      <c r="F264" s="23" t="s">
-        <v>865</v>
-      </c>
-      <c r="G264" s="24" t="s">
-        <v>866</v>
-      </c>
-      <c r="H264" s="24" t="s">
-        <v>867</v>
-      </c>
-      <c r="I264" s="24" t="s">
-        <v>868</v>
+      <c r="F264" s="35" t="s">
+        <v>926</v>
+      </c>
+      <c r="G264" s="34" t="s">
+        <v>927</v>
+      </c>
+      <c r="H264" s="34" t="s">
+        <v>924</v>
+      </c>
+      <c r="I264" s="34" t="s">
+        <v>925</v>
       </c>
       <c r="J264" s="25" t="s">
         <v>488</v>
@@ -16955,13 +16958,13 @@
         <v>488</v>
       </c>
       <c r="N264" s="25" t="s">
-        <v>869</v>
+        <v>928</v>
       </c>
       <c r="O264" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P264" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q264" s="25" t="s">
         <v>826</v>
@@ -16985,20 +16988,20 @@
       <c r="D265" s="21" t="s">
         <v>556</v>
       </c>
-      <c r="E265" s="22" t="s">
+      <c r="E265" s="38" t="s">
         <v>557</v>
       </c>
-      <c r="F265" s="23" t="s">
-        <v>870</v>
-      </c>
-      <c r="G265" s="24" t="s">
-        <v>871</v>
-      </c>
-      <c r="H265" s="24" t="s">
-        <v>872</v>
-      </c>
-      <c r="I265" s="24" t="s">
-        <v>873</v>
+      <c r="F265" s="35" t="s">
+        <v>907</v>
+      </c>
+      <c r="G265" s="34" t="s">
+        <v>908</v>
+      </c>
+      <c r="H265" s="34" t="s">
+        <v>909</v>
+      </c>
+      <c r="I265" s="34" t="s">
+        <v>910</v>
       </c>
       <c r="J265" s="25" t="s">
         <v>488</v>
@@ -17011,13 +17014,13 @@
         <v>488</v>
       </c>
       <c r="N265" s="25" t="s">
-        <v>874</v>
+        <v>841</v>
       </c>
       <c r="O265" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P265" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q265" s="25" t="s">
         <v>826</v>
@@ -17044,17 +17047,17 @@
       <c r="E266" s="22" t="s">
         <v>559</v>
       </c>
-      <c r="F266" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="G266" s="24" t="s">
-        <v>876</v>
-      </c>
-      <c r="H266" s="24" t="s">
-        <v>877</v>
-      </c>
-      <c r="I266" s="24" t="s">
-        <v>878</v>
+      <c r="F266" s="35" t="s">
+        <v>913</v>
+      </c>
+      <c r="G266" s="34" t="s">
+        <v>914</v>
+      </c>
+      <c r="H266" s="34" t="s">
+        <v>911</v>
+      </c>
+      <c r="I266" s="34" t="s">
+        <v>912</v>
       </c>
       <c r="J266" s="25" t="s">
         <v>488</v>
@@ -17067,13 +17070,13 @@
         <v>488</v>
       </c>
       <c r="N266" s="25" t="s">
-        <v>879</v>
+        <v>842</v>
       </c>
       <c r="O266" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P266" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q266" s="25" t="s">
         <v>826</v>
@@ -17100,17 +17103,17 @@
       <c r="E267" s="22" t="s">
         <v>561</v>
       </c>
-      <c r="F267" s="23" t="s">
-        <v>880</v>
-      </c>
-      <c r="G267" s="24" t="s">
-        <v>881</v>
-      </c>
-      <c r="H267" s="24" t="s">
-        <v>882</v>
-      </c>
-      <c r="I267" s="24" t="s">
-        <v>883</v>
+      <c r="F267" s="35" t="s">
+        <v>915</v>
+      </c>
+      <c r="G267" s="34" t="s">
+        <v>916</v>
+      </c>
+      <c r="H267" s="34" t="s">
+        <v>917</v>
+      </c>
+      <c r="I267" s="34" t="s">
+        <v>918</v>
       </c>
       <c r="J267" s="25" t="s">
         <v>488</v>
@@ -17123,13 +17126,13 @@
         <v>488</v>
       </c>
       <c r="N267" s="25" t="s">
-        <v>884</v>
+        <v>843</v>
       </c>
       <c r="O267" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P267" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q267" s="25" t="s">
         <v>826</v>
@@ -17156,17 +17159,17 @@
       <c r="E268" s="22" t="s">
         <v>563</v>
       </c>
-      <c r="F268" s="23" t="s">
-        <v>885</v>
-      </c>
-      <c r="G268" s="24" t="s">
-        <v>886</v>
-      </c>
-      <c r="H268" s="24" t="s">
-        <v>887</v>
-      </c>
-      <c r="I268" s="24" t="s">
-        <v>888</v>
+      <c r="F268" s="35" t="s">
+        <v>919</v>
+      </c>
+      <c r="G268" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="H268" s="34" t="s">
+        <v>921</v>
+      </c>
+      <c r="I268" s="34" t="s">
+        <v>922</v>
       </c>
       <c r="J268" s="25" t="s">
         <v>488</v>
@@ -17179,13 +17182,13 @@
         <v>488</v>
       </c>
       <c r="N268" s="25" t="s">
-        <v>889</v>
+        <v>844</v>
       </c>
       <c r="O268" s="25" t="s">
         <v>488</v>
       </c>
       <c r="P268" s="25" t="s">
-        <v>854</v>
+        <v>838</v>
       </c>
       <c r="Q268" s="25" t="s">
         <v>826</v>
@@ -17220,7 +17223,7 @@
         <v>828</v>
       </c>
       <c r="K269" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L269" s="25"/>
       <c r="M269" s="25"/>
@@ -17258,7 +17261,7 @@
         <v>828</v>
       </c>
       <c r="K270" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L270" s="25"/>
       <c r="M270" s="25"/>
@@ -17296,7 +17299,7 @@
         <v>828</v>
       </c>
       <c r="K271" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L271" s="25"/>
       <c r="M271" s="25"/>
@@ -17334,7 +17337,7 @@
         <v>828</v>
       </c>
       <c r="K272" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L272" s="25"/>
       <c r="M272" s="25"/>
@@ -17372,7 +17375,7 @@
         <v>828</v>
       </c>
       <c r="K273" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L273" s="25"/>
       <c r="M273" s="25"/>
@@ -17410,7 +17413,7 @@
         <v>828</v>
       </c>
       <c r="K274" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L274" s="25"/>
       <c r="M274" s="25"/>
@@ -17448,7 +17451,7 @@
         <v>828</v>
       </c>
       <c r="K275" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L275" s="25"/>
       <c r="M275" s="25"/>
@@ -17486,7 +17489,7 @@
         <v>828</v>
       </c>
       <c r="K276" s="25" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="L276" s="25"/>
       <c r="M276" s="25"/>
@@ -30437,7 +30440,6 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="LDO"/>
         <filter val="RAD"/>
       </filters>
     </filterColumn>
@@ -33198,6 +33200,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA9DE3DB3C6091468D1D4005047F3381" ma:contentTypeVersion="10" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="f61d519a90cb3d2441383036b3cbbf0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ae8219d-8505-4e64-b47a-e5e02bd99ff8" xmlns:ns3="b6c6c545-4433-4453-a388-ae81a1a09069" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b500fd2dfba25c9cd9d811d5149d18" ns2:_="" ns3:_="">
     <xsd:import namespace="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
@@ -33402,15 +33413,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -33423,6 +33425,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0A55748-B993-405F-A7B1-83B812C422D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ACD8119-0795-4CC2-832D-F23B6321E24B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33441,21 +33451,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0A55748-B993-405F-A7B1-83B812C422D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB6DE5B0-8491-4C0A-95CF-DF2DFEFABE1F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b6c6c545-4433-4453-a388-ae81a1a09069"/>
+    <ds:schemaRef ds:uri="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
-    <ds:schemaRef ds:uri="b6c6c545-4433-4453-a388-ae81a1a09069"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>